<commit_message>
working with 2 chrom suis1
</commit_message>
<xml_diff>
--- a/dependencies/brucella/suis1/script_dependents/DefiningSNPsGroupDesignations.xlsx
+++ b/dependencies/brucella/suis1/script_dependents/DefiningSNPsGroupDesignations.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10814"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/root/TStuber/Results/brucella/suis1/script_dependents/python/script2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tstuber/workspace/vSNP/dependencies/brucella/suis1/script_dependents/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6530993-38DF-1E4F-A9C6-7065502868E1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="460" windowWidth="21600" windowHeight="17460"/>
+    <workbookView xWindow="1740" yWindow="460" windowWidth="29660" windowHeight="22160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -113,88 +114,88 @@
     <t>Bsuis1-11C3</t>
   </si>
   <si>
-    <t>gi|384223698|ref|NC_017251.1|-213522</t>
-  </si>
-  <si>
-    <t>gi|384223698|ref|NC_017251.1|-1146371</t>
-  </si>
-  <si>
-    <t>gi|384223698|ref|NC_017251.1|-549890</t>
-  </si>
-  <si>
-    <t>gi|384223698|ref|NC_017251.1|-1184227</t>
-  </si>
-  <si>
-    <t>gi|384223698|ref|NC_017251.1|-1245156</t>
-  </si>
-  <si>
-    <t>gi|384223698|ref|NC_017251.1|-994359</t>
-  </si>
-  <si>
-    <t>gi|384223698|ref|NC_017251.1|-1088654</t>
-  </si>
-  <si>
-    <t>gi|384222553|ref|NC_017250.1|-1173757</t>
-  </si>
-  <si>
-    <t>gi|384222553|ref|NC_017250.1|-241603</t>
-  </si>
-  <si>
-    <t>gi|384222553|ref|NC_017250.1|-1013589</t>
-  </si>
-  <si>
-    <t>gi|384222553|ref|NC_017250.1|-1025446</t>
-  </si>
-  <si>
-    <t>gi|384222553|ref|NC_017250.1|-1020241</t>
-  </si>
-  <si>
-    <t>gi|384222553|ref|NC_017250.1|-1175324</t>
-  </si>
-  <si>
-    <t>gi|384222553|ref|NC_017250.1|-291907</t>
-  </si>
-  <si>
-    <t>gi|384222553|ref|NC_017250.1|-1197913</t>
-  </si>
-  <si>
-    <t>gi|384222553|ref|NC_017250.1|-1016576</t>
-  </si>
-  <si>
-    <t>gi|384222553|ref|NC_017250.1|-264518</t>
-  </si>
-  <si>
-    <t>gi|384222553|ref|NC_017250.1|-1014292</t>
-  </si>
-  <si>
-    <t>gi|384222553|ref|NC_017250.1|-1048661</t>
-  </si>
-  <si>
-    <t>gi|384222553|ref|NC_017250.1|-1072841</t>
-  </si>
-  <si>
-    <t>gi|384222553|ref|NC_017250.1|-1099151</t>
-  </si>
-  <si>
-    <t>gi|384222553|ref|NC_017250.1|-1167451</t>
-  </si>
-  <si>
-    <t>gi|384222553|ref|NC_017250.1|-1011109</t>
-  </si>
-  <si>
-    <t>gi|384222553|ref|NC_017250.1|-1035261</t>
-  </si>
-  <si>
-    <t>gi|384222553|ref|NC_017250.1|-1147663</t>
-  </si>
-  <si>
-    <t>gi|384222553|ref|NC_017250.1|-1195126</t>
+    <t>NC_017251.1-213522</t>
+  </si>
+  <si>
+    <t>NC_017251.1-1146371</t>
+  </si>
+  <si>
+    <t>NC_017251.1-549890</t>
+  </si>
+  <si>
+    <t>NC_017251.1-1184227</t>
+  </si>
+  <si>
+    <t>NC_017251.1-1245156</t>
+  </si>
+  <si>
+    <t>NC_017251.1-994359</t>
+  </si>
+  <si>
+    <t>NC_017251.1-1088654</t>
+  </si>
+  <si>
+    <t>NC_017250.1-1173757</t>
+  </si>
+  <si>
+    <t>NC_017250.1-241603</t>
+  </si>
+  <si>
+    <t>NC_017250.1-1013589</t>
+  </si>
+  <si>
+    <t>NC_017250.1-1025446</t>
+  </si>
+  <si>
+    <t>NC_017250.1-1020241</t>
+  </si>
+  <si>
+    <t>NC_017250.1-1175324</t>
+  </si>
+  <si>
+    <t>NC_017250.1-291907</t>
+  </si>
+  <si>
+    <t>NC_017250.1-1197913</t>
+  </si>
+  <si>
+    <t>NC_017250.1-1016576</t>
+  </si>
+  <si>
+    <t>NC_017250.1-264518</t>
+  </si>
+  <si>
+    <t>NC_017250.1-1014292</t>
+  </si>
+  <si>
+    <t>NC_017250.1-1048661</t>
+  </si>
+  <si>
+    <t>NC_017250.1-1072841</t>
+  </si>
+  <si>
+    <t>NC_017250.1-1099151</t>
+  </si>
+  <si>
+    <t>NC_017250.1-1167451</t>
+  </si>
+  <si>
+    <t>NC_017250.1-1011109</t>
+  </si>
+  <si>
+    <t>NC_017250.1-1035261</t>
+  </si>
+  <si>
+    <t>NC_017250.1-1147663</t>
+  </si>
+  <si>
+    <t>NC_017250.1-1195126</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -765,12 +766,13 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="110">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1183,12 +1185,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
+      <selection pane="bottomLeft" activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1210,7 +1212,7 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1218,7 +1220,7 @@
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1226,7 +1228,7 @@
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1234,7 +1236,7 @@
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1242,7 +1244,7 @@
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1250,7 +1252,7 @@
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="3" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1258,7 +1260,7 @@
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="3" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1266,7 +1268,7 @@
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="3" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1274,7 +1276,7 @@
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="3" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1282,7 +1284,7 @@
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="3" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1290,7 +1292,7 @@
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="3" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1298,7 +1300,7 @@
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="3" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1306,7 +1308,7 @@
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="3" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1314,7 +1316,7 @@
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="3" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1322,7 +1324,7 @@
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="3" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1330,7 +1332,7 @@
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="3" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1338,7 +1340,7 @@
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="3" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1346,7 +1348,7 @@
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="3" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1354,7 +1356,7 @@
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="3" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1362,7 +1364,7 @@
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="3" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1370,7 +1372,7 @@
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="3" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1378,7 +1380,7 @@
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="3" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1386,7 +1388,7 @@
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="3" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1394,7 +1396,7 @@
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="3" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1402,7 +1404,7 @@
       <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="3" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1410,7 +1412,7 @@
       <c r="A27" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="3" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated af2122 and suis1 dependencies with no gi
</commit_message>
<xml_diff>
--- a/dependencies/brucella/suis1/script_dependents/DefiningSNPsGroupDesignations.xlsx
+++ b/dependencies/brucella/suis1/script_dependents/DefiningSNPsGroupDesignations.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10814"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/root/TStuber/Results/brucella/suis1/script_dependents/python/script2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tstuber/workspace/vSNP/dependencies/brucella/suis1/script_dependents/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6530993-38DF-1E4F-A9C6-7065502868E1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="460" windowWidth="21600" windowHeight="17460"/>
+    <workbookView xWindow="1740" yWindow="460" windowWidth="29660" windowHeight="22160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -113,88 +114,88 @@
     <t>Bsuis1-11C3</t>
   </si>
   <si>
-    <t>gi|384223698|ref|NC_017251.1|-213522</t>
-  </si>
-  <si>
-    <t>gi|384223698|ref|NC_017251.1|-1146371</t>
-  </si>
-  <si>
-    <t>gi|384223698|ref|NC_017251.1|-549890</t>
-  </si>
-  <si>
-    <t>gi|384223698|ref|NC_017251.1|-1184227</t>
-  </si>
-  <si>
-    <t>gi|384223698|ref|NC_017251.1|-1245156</t>
-  </si>
-  <si>
-    <t>gi|384223698|ref|NC_017251.1|-994359</t>
-  </si>
-  <si>
-    <t>gi|384223698|ref|NC_017251.1|-1088654</t>
-  </si>
-  <si>
-    <t>gi|384222553|ref|NC_017250.1|-1173757</t>
-  </si>
-  <si>
-    <t>gi|384222553|ref|NC_017250.1|-241603</t>
-  </si>
-  <si>
-    <t>gi|384222553|ref|NC_017250.1|-1013589</t>
-  </si>
-  <si>
-    <t>gi|384222553|ref|NC_017250.1|-1025446</t>
-  </si>
-  <si>
-    <t>gi|384222553|ref|NC_017250.1|-1020241</t>
-  </si>
-  <si>
-    <t>gi|384222553|ref|NC_017250.1|-1175324</t>
-  </si>
-  <si>
-    <t>gi|384222553|ref|NC_017250.1|-291907</t>
-  </si>
-  <si>
-    <t>gi|384222553|ref|NC_017250.1|-1197913</t>
-  </si>
-  <si>
-    <t>gi|384222553|ref|NC_017250.1|-1016576</t>
-  </si>
-  <si>
-    <t>gi|384222553|ref|NC_017250.1|-264518</t>
-  </si>
-  <si>
-    <t>gi|384222553|ref|NC_017250.1|-1014292</t>
-  </si>
-  <si>
-    <t>gi|384222553|ref|NC_017250.1|-1048661</t>
-  </si>
-  <si>
-    <t>gi|384222553|ref|NC_017250.1|-1072841</t>
-  </si>
-  <si>
-    <t>gi|384222553|ref|NC_017250.1|-1099151</t>
-  </si>
-  <si>
-    <t>gi|384222553|ref|NC_017250.1|-1167451</t>
-  </si>
-  <si>
-    <t>gi|384222553|ref|NC_017250.1|-1011109</t>
-  </si>
-  <si>
-    <t>gi|384222553|ref|NC_017250.1|-1035261</t>
-  </si>
-  <si>
-    <t>gi|384222553|ref|NC_017250.1|-1147663</t>
-  </si>
-  <si>
-    <t>gi|384222553|ref|NC_017250.1|-1195126</t>
+    <t>NC_017251.1-213522</t>
+  </si>
+  <si>
+    <t>NC_017251.1-1146371</t>
+  </si>
+  <si>
+    <t>NC_017251.1-549890</t>
+  </si>
+  <si>
+    <t>NC_017251.1-1184227</t>
+  </si>
+  <si>
+    <t>NC_017251.1-1245156</t>
+  </si>
+  <si>
+    <t>NC_017251.1-994359</t>
+  </si>
+  <si>
+    <t>NC_017251.1-1088654</t>
+  </si>
+  <si>
+    <t>NC_017250.1-1173757</t>
+  </si>
+  <si>
+    <t>NC_017250.1-241603</t>
+  </si>
+  <si>
+    <t>NC_017250.1-1013589</t>
+  </si>
+  <si>
+    <t>NC_017250.1-1025446</t>
+  </si>
+  <si>
+    <t>NC_017250.1-1020241</t>
+  </si>
+  <si>
+    <t>NC_017250.1-1175324</t>
+  </si>
+  <si>
+    <t>NC_017250.1-291907</t>
+  </si>
+  <si>
+    <t>NC_017250.1-1197913</t>
+  </si>
+  <si>
+    <t>NC_017250.1-1016576</t>
+  </si>
+  <si>
+    <t>NC_017250.1-264518</t>
+  </si>
+  <si>
+    <t>NC_017250.1-1014292</t>
+  </si>
+  <si>
+    <t>NC_017250.1-1048661</t>
+  </si>
+  <si>
+    <t>NC_017250.1-1072841</t>
+  </si>
+  <si>
+    <t>NC_017250.1-1099151</t>
+  </si>
+  <si>
+    <t>NC_017250.1-1167451</t>
+  </si>
+  <si>
+    <t>NC_017250.1-1011109</t>
+  </si>
+  <si>
+    <t>NC_017250.1-1035261</t>
+  </si>
+  <si>
+    <t>NC_017250.1-1147663</t>
+  </si>
+  <si>
+    <t>NC_017250.1-1195126</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -765,12 +766,13 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="110">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1183,12 +1185,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
+      <selection pane="bottomLeft" activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1210,7 +1212,7 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1218,7 +1220,7 @@
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1226,7 +1228,7 @@
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1234,7 +1236,7 @@
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1242,7 +1244,7 @@
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1250,7 +1252,7 @@
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="3" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1258,7 +1260,7 @@
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="3" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1266,7 +1268,7 @@
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="3" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1274,7 +1276,7 @@
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="3" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1282,7 +1284,7 @@
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="3" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1290,7 +1292,7 @@
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="3" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1298,7 +1300,7 @@
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="3" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1306,7 +1308,7 @@
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="3" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1314,7 +1316,7 @@
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="3" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1322,7 +1324,7 @@
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="3" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1330,7 +1332,7 @@
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="3" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1338,7 +1340,7 @@
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="3" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1346,7 +1348,7 @@
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="3" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1354,7 +1356,7 @@
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="3" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1362,7 +1364,7 @@
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="3" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1370,7 +1372,7 @@
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="3" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1378,7 +1380,7 @@
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="3" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1386,7 +1388,7 @@
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="3" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1394,7 +1396,7 @@
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="3" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1402,7 +1404,7 @@
       <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="3" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1410,7 +1412,7 @@
       <c r="A27" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="3" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>